<commit_message>
Update quiz-app subproject status and modify results data structure
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgson\Desktop\SakshiSoni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EF2510-739F-4819-A16E-4EEA38462484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78629635-2429-442B-B12C-0D2F36078D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Question Text</t>
   </si>
@@ -45,29 +45,14 @@
     <t>Correct Option Index</t>
   </si>
   <si>
-    <t>What is 2 + 2?</t>
-  </si>
-  <si>
-    <t>Capital of France?</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>Paris</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>London</t>
+    <t>2+2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,32 +60,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FFF3F4F6"/>
-      <name val="Source Sans Pro"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFF3F4F6"/>
-      <name val="Source Sans Pro"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF111827"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -115,14 +81,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,72 +363,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="42.36328125" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="36" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="24" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="E2">
         <v>4</v>
       </c>
-      <c r="D2" s="2">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="24" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
+      <c r="F2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>